<commit_message>
Añadir link del servo
</commit_message>
<xml_diff>
--- a/docs/gestion/monetaria.xlsx
+++ b/docs/gestion/monetaria.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t xml:space="preserve">Presupuesto</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t xml:space="preserve">Acelerómetro de 3 ejes, resolución 13 bits hasta 16G, I2C y SPI comms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM-S2309S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servomotor, servo, motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servo chiquito plasticucho de 150º de apertura. Tiene cable feedback.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://servodatabase.com/servo/springrc/sm-s2309s</t>
   </si>
 </sst>
 </file>
@@ -421,10 +433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -434,6 +446,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="60.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.45"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,6 +468,9 @@
       <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -515,6 +531,23 @@
       </c>
       <c r="E6" s="0" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadida compra de Steppers al excel
</commit_message>
<xml_diff>
--- a/docs/gestion/monetaria.xlsx
+++ b/docs/gestion/monetaria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Hueso Béjar\Desktop\Subj_Robotics\docs\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Hueso Béjar\Desktop\3\2º Cuatrimestre\Robótica\2_Trabajo\Subj_Robotics\docs\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12676A63-358D-4A5C-B55C-1FCA6769B87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7DA8E1-F6FB-4A88-85C5-88DFF519A00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35070" yWindow="2070" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>INVENTARIO</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/dp/B07SWYFCQV?smid=A3LC78H97WEBWA&amp;ref_=chk_typ_imgToDp&amp;th=1</t>
+  </si>
+  <si>
+    <t>Motor 17HS4401</t>
+  </si>
+  <si>
+    <t>Motor, Stepper</t>
+  </si>
+  <si>
+    <t>Motor Paso Paso Nema 17</t>
   </si>
 </sst>
 </file>
@@ -552,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -582,6 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -998,7 +1011,7 @@
       </c>
       <c r="C3" s="16">
         <f>SUM(Compras!D3:D27)</f>
-        <v>12.49</v>
+        <v>54.22</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1007,7 +1020,7 @@
       </c>
       <c r="C4" s="18">
         <f>C2-C3</f>
-        <v>187.51</v>
+        <v>145.78</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1050,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1076,9 +1089,15 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="29">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="9">
+        <v>41.73</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="7"/>
@@ -1199,6 +1218,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" location="Inventario_cero_coste!B10" display="Inventario_cero_coste!B10" xr:uid="{40E4946C-C14A-4825-86CB-A0E668F81A02}"/>
+    <hyperlink ref="B4" location="Inventario_cero_coste!B11" display="Inventario_cero_coste!B11" xr:uid="{D03FE732-52E1-41E6-9D52-C171618E412B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1214,7 +1234,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="20" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1395,7 +1415,7 @@
         <v>14</v>
       </c>
       <c r="H9" s="8"/>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1425,13 +1445,23 @@
       <c r="B11" s="7">
         <v>9</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="19"/>
+      <c r="I11" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="7">
@@ -1629,9 +1659,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1" display="https://www.amazon.es/HiLetgo-WXD3-13-2W-Multi-Turn-Wirewound-Potentiometer/dp/B07ZZ1KHVL/ref=sr_1_3?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=1AXCB2NZAYA3O&amp;keywords=potentiometer+multiturn&amp;qid=1681151469&amp;sprefix=potentiometer+multiturn%2Caps%2C130&amp;sr=8-3" xr:uid="{9780FAFF-7904-4210-9DE6-57F35D220F48}"/>
+    <hyperlink ref="I11" r:id="rId2" xr:uid="{C7096641-08C1-416B-8911-CFD0EF173D80}"/>
+    <hyperlink ref="I8" r:id="rId3" xr:uid="{58111E8B-6628-422E-BE04-CF465EC8386E}"/>
+    <hyperlink ref="I9" r:id="rId4" xr:uid="{8C0F92A6-3E72-443F-BAEF-B5691E18103B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Añadida la compra de servos al excel
</commit_message>
<xml_diff>
--- a/docs/gestion/monetaria.xlsx
+++ b/docs/gestion/monetaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Hueso Béjar\Desktop\3\2º Cuatrimestre\Robótica\2_Trabajo\Subj_Robotics\docs\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpuya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7DA8E1-F6FB-4A88-85C5-88DFF519A00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B36866-33F0-468B-ADA0-6F695C4FF8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35070" yWindow="2070" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -38,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -186,6 +175,21 @@
   </si>
   <si>
     <t>Motor Paso Paso Nema 17</t>
+  </si>
+  <si>
+    <t>https://tienda.bricogeek.com/servomotores/1320-mini-servo-feetech-3-5kg-ft1117m-fb-con-feedback.html</t>
+  </si>
+  <si>
+    <t>Fran</t>
+  </si>
+  <si>
+    <t>Servomotor realimentado</t>
+  </si>
+  <si>
+    <t>FT1117M-FB</t>
+  </si>
+  <si>
+    <t>Servomotores realimentados de 3.5kg·cm</t>
   </si>
 </sst>
 </file>
@@ -980,9 +984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1011,7 +1015,7 @@
       </c>
       <c r="C3" s="16">
         <f>SUM(Compras!D3:D27)</f>
-        <v>54.22</v>
+        <v>80.180000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1020,7 +1024,7 @@
       </c>
       <c r="C4" s="18">
         <f>C2-C3</f>
-        <v>145.78</v>
+        <v>119.82</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1054,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1100,9 +1104,15 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="29">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="9">
+        <v>25.96</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="7"/>
@@ -1219,6 +1229,7 @@
   <hyperlinks>
     <hyperlink ref="B3" location="Inventario_cero_coste!B10" display="Inventario_cero_coste!B10" xr:uid="{40E4946C-C14A-4825-86CB-A0E668F81A02}"/>
     <hyperlink ref="B4" location="Inventario_cero_coste!B11" display="Inventario_cero_coste!B11" xr:uid="{D03FE732-52E1-41E6-9D52-C171618E412B}"/>
+    <hyperlink ref="B5" location="Inventario_cero_coste!B10" display="10" xr:uid="{CAEC3928-D5D5-432E-9BF3-D31161648768}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1233,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,13 +1478,23 @@
       <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="H12" s="8"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="7">
@@ -1662,9 +1683,10 @@
     <hyperlink ref="I11" r:id="rId2" xr:uid="{C7096641-08C1-416B-8911-CFD0EF173D80}"/>
     <hyperlink ref="I8" r:id="rId3" xr:uid="{58111E8B-6628-422E-BE04-CF465EC8386E}"/>
     <hyperlink ref="I9" r:id="rId4" xr:uid="{8C0F92A6-3E72-443F-BAEF-B5691E18103B}"/>
+    <hyperlink ref="I12" r:id="rId5" xr:uid="{6B27758C-AFB0-464D-A523-F8F57545D44B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Carpeta CAD y gestión económica actualizada
</commit_message>
<xml_diff>
--- a/docs/gestion/monetaria.xlsx
+++ b/docs/gestion/monetaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fpuya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Hueso Béjar\Desktop\3\2º Cuatrimestre\Robótica\2_Trabajo\Subj_Robotics\docs\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B36866-33F0-468B-ADA0-6F695C4FF8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89958311-B05D-4A95-8684-A8D170B1AF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="180" windowWidth="21600" windowHeight="8565" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -27,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>Presupuesto</t>
   </si>
@@ -190,6 +201,57 @@
   </si>
   <si>
     <t>Servomotores realimentados de 3.5kg·cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRV8825 </t>
+  </si>
+  <si>
+    <t>Módulo controlador Stepper</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/dp/B07YWV6W4W?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Bolas rodamientos</t>
+  </si>
+  <si>
+    <t>Bolas rodamientos 560 piezas, 11 tamaños</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/dp/B094346M9W?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Hilo tórico</t>
+  </si>
+  <si>
+    <t>Hilo tórico de caucho 2.5 mm de diámetro, 1 m</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/dp/B0BD5P49Q8?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>https://www.amazon.es/dp/B0BB15P6DL?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Cubrecables</t>
+  </si>
+  <si>
+    <t>Cubrecables 13-20 mm de diámetro, 3 m</t>
+  </si>
+  <si>
+    <t>Mecánica</t>
+  </si>
+  <si>
+    <t>Elementos mecánicos</t>
+  </si>
+  <si>
+    <t>2 Correas dentadas GT2, 5 rodamientos lineales, 2 varillas lisas, 3 poleas GT2</t>
+  </si>
+  <si>
+    <t>https://www.hta3d.com</t>
+  </si>
+  <si>
+    <t>5 Módulos controlador para stepper</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1077,7 @@
       </c>
       <c r="C3" s="16">
         <f>SUM(Compras!D3:D27)</f>
-        <v>80.180000000000007</v>
+        <v>161.64000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1024,7 +1086,7 @@
       </c>
       <c r="C4" s="18">
         <f>C2-C3</f>
-        <v>119.82</v>
+        <v>38.359999999999985</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1115,34 +1177,70 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="29">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="9">
+        <v>22.49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
+      <c r="B7" s="29">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="9">
+        <v>13.99</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="29">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6.95</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="29">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="9">
+        <v>6.95</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="29">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="9">
+        <v>8.99</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="29">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9">
+        <v>22.09</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
@@ -1230,6 +1328,12 @@
     <hyperlink ref="B3" location="Inventario_cero_coste!B10" display="Inventario_cero_coste!B10" xr:uid="{40E4946C-C14A-4825-86CB-A0E668F81A02}"/>
     <hyperlink ref="B4" location="Inventario_cero_coste!B11" display="Inventario_cero_coste!B11" xr:uid="{D03FE732-52E1-41E6-9D52-C171618E412B}"/>
     <hyperlink ref="B5" location="Inventario_cero_coste!B10" display="10" xr:uid="{CAEC3928-D5D5-432E-9BF3-D31161648768}"/>
+    <hyperlink ref="B6" location="Inventario_cero_coste!B13" display="11" xr:uid="{B09DFD93-BFE3-430B-8082-BEA43CA80570}"/>
+    <hyperlink ref="B7" location="Inventario_cero_coste!B14" display="12" xr:uid="{7FDC4A67-3B22-46CA-A184-7F4F5154B538}"/>
+    <hyperlink ref="B8" location="Compras!B15" display="13" xr:uid="{8D2DB229-F9EA-48B5-9F65-B6CA7516F613}"/>
+    <hyperlink ref="B9" location="Inventario_cero_coste!B16" display="15" xr:uid="{75C67713-5E4F-4558-9D3F-6E4D8F5C45CF}"/>
+    <hyperlink ref="B10" location="Inventario_cero_coste!B17" display="15" xr:uid="{15E04807-0307-4F8E-A597-E719D9183F3D}"/>
+    <hyperlink ref="B11" location="Inventario_cero_coste!B18" display="16" xr:uid="{5743901C-D7A5-49EF-93D6-6CC0AF35D088}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1244,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1500,73 +1604,133 @@
       <c r="B13" s="7">
         <v>11</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="19"/>
+      <c r="I13" s="20" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="7">
         <v>12</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="7">
         <v>13</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="7">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="7">
         <v>15</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="7">
         <v>16</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="7">
@@ -1684,9 +1848,15 @@
     <hyperlink ref="I8" r:id="rId3" xr:uid="{58111E8B-6628-422E-BE04-CF465EC8386E}"/>
     <hyperlink ref="I9" r:id="rId4" xr:uid="{8C0F92A6-3E72-443F-BAEF-B5691E18103B}"/>
     <hyperlink ref="I12" r:id="rId5" xr:uid="{6B27758C-AFB0-464D-A523-F8F57545D44B}"/>
+    <hyperlink ref="I13" r:id="rId6" xr:uid="{F9FF7DC1-F8C0-40BE-8454-38FFD4D60377}"/>
+    <hyperlink ref="I14" r:id="rId7" xr:uid="{80658A55-34A9-44E4-B309-D246142E107E}"/>
+    <hyperlink ref="I15" r:id="rId8" xr:uid="{E516B866-7FF5-4D42-A240-1059B6384E3D}"/>
+    <hyperlink ref="I16" r:id="rId9" xr:uid="{CD880D5D-F54D-48B1-B27D-B5C312D1544F}"/>
+    <hyperlink ref="I17" r:id="rId10" xr:uid="{DF35E984-2B86-46BD-A3A8-DE38A765B987}"/>
+    <hyperlink ref="I18" r:id="rId11" xr:uid="{4AC66E93-BC2D-4F91-893C-02B48D6C015D}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>